<commit_message>
Ajuste carga de catalogos
</commit_message>
<xml_diff>
--- a/src/assets/files/14.Responsables.xlsx
+++ b/src/assets/files/14.Responsables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brquezada\Documents\projects\frontEnd\gui-mst-adt-web\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgutierrez\Documents\proyectos\angular\demos\trabajo-social-adt\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD05EF2-F882-422B-8E4A-0A3FC8E5FD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867FEF23-DB5C-4DA6-8BB2-118FBEC2F557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{81DE2BF2-5820-420D-8D45-6D412EA3A9D3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{81DE2BF2-5820-420D-8D45-6D412EA3A9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="C_personal" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>PRIMER APELLIDO</t>
   </si>
@@ -90,9 +90,6 @@
     <t>TURNO</t>
   </si>
   <si>
-    <t>Trab_Social_05</t>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
@@ -115,6 +112,15 @@
   </si>
   <si>
     <t>Turno</t>
+  </si>
+  <si>
+    <t>SERVICIO/ESPECIALIDAD</t>
+  </si>
+  <si>
+    <t>Servicios de Enlace</t>
+  </si>
+  <si>
+    <t>Trab_Social_02</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -168,6 +174,10 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,33 +533,33 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>987654321</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
       </c>
       <c r="I2">
         <v>987654321</v>
@@ -983,10 +993,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8511366-658D-4A34-8384-75E1F6FA7EAE}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -997,7 +1007,7 @@
     <col min="4" max="4" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1010,613 +1020,25 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>987654321</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B3,C_personal!A5:G103,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B4,C_personal!A6:G104,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B5,C_personal!A7:G105,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B6,C_personal!A8:G106,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B7,C_personal!A9:G107,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B8,C_personal!A10:G108,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B9,C_personal!A11:G109,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B10,C_personal!A12:G110,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B11,C_personal!A13:G111,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B12,C_personal!A14:G112,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B13,C_personal!A15:G113,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B14,C_personal!A16:G114,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B15,C_personal!A17:G115,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B16,C_personal!A18:G116,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B17,C_personal!A19:G117,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B18,C_personal!A20:G118,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B19,C_personal!A21:G119,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B20,C_personal!A22:G120,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B21,C_personal!A23:G121,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B22,C_personal!A24:G122,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B23,C_personal!A25:G123,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B24,C_personal!A26:G124,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B25,C_personal!A27:G125,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B26,C_personal!A28:G126,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B27,C_personal!A29:G127,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B28,C_personal!A30:G128,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B29,C_personal!A31:G129,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B30,C_personal!A32:G130,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B31,C_personal!A33:G131,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B32,C_personal!A34:G132,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B33,C_personal!A35:G133,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B34,C_personal!A36:G134,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B35,C_personal!A37:G135,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B36,C_personal!A38:G136,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B37,C_personal!A39:G137,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B38,C_personal!A40:G138,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B39,C_personal!A41:G139,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B40,C_personal!A42:G140,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B41,C_personal!A43:G141,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B42,C_personal!A44:G142,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B43,C_personal!A45:G143,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B44,C_personal!A46:G144,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B45,C_personal!A47:G145,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B46,C_personal!A48:G146,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B47,C_personal!A49:G147,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B48,C_personal!A50:G148,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B49,C_personal!A51:G149,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B50,C_personal!A52:G150,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B51,C_personal!A53:G151,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B52,C_personal!A54:G152,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B53,C_personal!A55:G153,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B54,C_personal!A56:G154,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B55,C_personal!A57:G155,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B56,C_personal!A58:G156,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B57,C_personal!A59:G157,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B58,C_personal!A60:G158,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B59,C_personal!A61:G159,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B60,C_personal!A62:G160,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B61,C_personal!A63:G161,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B62,C_personal!A64:G162,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B63,C_personal!A65:G163,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B64,C_personal!A66:G164,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B65,C_personal!A67:G165,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B66,C_personal!A68:G166,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B67,C_personal!A69:G167,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B68,C_personal!A70:G168,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B69,C_personal!A71:G169,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B70,C_personal!A72:G170,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B71,C_personal!A73:G171,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B72,C_personal!A74:G172,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B73,C_personal!A75:G173,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B74,C_personal!A76:G174,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B75,C_personal!A77:G175,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B76,C_personal!A78:G176,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B77,C_personal!A79:G177,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B78,C_personal!A80:G178,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B79,C_personal!A81:G179,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B80,C_personal!A82:G180,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B81,C_personal!A83:G181,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B82,C_personal!A84:G182,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B83,C_personal!A85:G183,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B84,C_personal!A86:G184,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B85,C_personal!A87:G185,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B86,C_personal!A88:G186,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B87,C_personal!A89:G187,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B88,C_personal!A90:G188,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B89,C_personal!A91:G189,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B90,C_personal!A92:G190,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B91,C_personal!A93:G191,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B92,C_personal!A94:G192,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B93,C_personal!A95:G193,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B94,C_personal!A96:G194,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B95,C_personal!A97:G195,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B96,C_personal!A98:G196,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B97,C_personal!A99:G197,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B98,C_personal!A100:G198,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B99,C_personal!A101:G199,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B100,C_personal!A102:G200,4),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A101" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(B101,C_personal!A103:G201,4),"")</f>
-        <v/>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix nombre campo ubicacion carga masiva
</commit_message>
<xml_diff>
--- a/src/assets/files/14.Responsables.xlsx
+++ b/src/assets/files/14.Responsables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545969FE-7AC8-49A5-8AE5-F3991DD4CECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3E99AC-D7C3-41E7-A802-444256499A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="864" windowWidth="21756" windowHeight="11304" activeTab="2" xr2:uid="{81DE2BF2-5820-420D-8D45-6D412EA3A9D3}"/>
+    <workbookView xWindow="-16183" yWindow="-2897" windowWidth="13423" windowHeight="5091" activeTab="2" xr2:uid="{81DE2BF2-5820-420D-8D45-6D412EA3A9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="C_personal" sheetId="1" r:id="rId1"/>
@@ -66,15 +66,9 @@
     <t>MATRICULA</t>
   </si>
   <si>
-    <t>UBICACIÓN</t>
-  </si>
-  <si>
     <t>TURNO</t>
   </si>
   <si>
-    <t>Trab_Social_05</t>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
@@ -271,6 +265,12 @@
   </si>
   <si>
     <t>Trabajo Social</t>
+  </si>
+  <si>
+    <t>DESCRIPCION COMPLETA DE UBICACIÓN</t>
+  </si>
+  <si>
+    <t>Trabajo_Social_01</t>
   </si>
 </sst>
 </file>
@@ -663,10 +663,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -678,325 +678,325 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>912083456</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>975432729</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>123453894</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>864263789</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>534283945</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>834417268</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>723498109</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>987938743</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>872345903</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>876234879</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>123257965</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>99091173</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1073,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,16 +1087,16 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1104,7 +1104,7 @@
         <v>912083456</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1113,7 +1113,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1141,6 +1141,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -1254,15 +1263,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA25A5CE-F7DC-4013-ADFC-9FDEC7F55BC7}">
   <ds:schemaRefs>
@@ -1273,6 +1273,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{429D3CF7-3DE4-46DF-9720-539F5F1E4406}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C479CB17-957D-44FB-B5DB-D83F812D9445}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1286,12 +1294,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{429D3CF7-3DE4-46DF-9720-539F5F1E4406}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>